<commit_message>
Dr.Netrapali Monday 10am, Annada moves to Tuesday
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amukh\OneDrive\Desktop\phdpathanagosthi23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEDCCE9-840B-4285-92CA-7A5D1E923AF6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DDAD526-0EED-4C3C-80C2-4BF418A21BE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5556" activeTab="1" xr2:uid="{C48E5C63-C363-4E87-BE09-F3DFD3C3D9D1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5556" activeTab="2" xr2:uid="{C48E5C63-C363-4E87-BE09-F3DFD3C3D9D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="66">
   <si>
     <t>8:30am</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>Do We Really Need Complicated Model Architectures for Temporal Networks?</t>
+  </si>
+  <si>
+    <t>Dr. Praneeth Netrapali</t>
   </si>
 </sst>
 </file>
@@ -265,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -290,6 +293,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -624,11 +630,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
@@ -737,11 +743,11 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
@@ -845,11 +851,11 @@
       <c r="C25" s="3"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
@@ -964,11 +970,11 @@
       <c r="C38" s="3"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
@@ -1072,11 +1078,11 @@
       <c r="C50" s="3"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
@@ -1180,11 +1186,11 @@
       <c r="C62" s="3"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="9" t="s">
+      <c r="A63" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B63" s="9"/>
-      <c r="C63" s="9"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="10"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
@@ -1292,10 +1298,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43BD2D15-4829-4DCB-88F7-A6DAAE9BCFF8}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1320,7 +1326,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>57</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1334,19 +1340,16 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="10"/>
+      <c r="A3" s="11"/>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>13</v>
+      <c r="C3" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="10"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1356,7 +1359,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1366,7 +1369,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="2" t="s">
         <v>20</v>
       </c>
@@ -1378,7 +1381,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
@@ -1390,7 +1393,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="2" t="s">
         <v>22</v>
       </c>
@@ -1400,7 +1403,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
@@ -1410,7 +1413,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="2" t="s">
         <v>24</v>
       </c>
@@ -1421,8 +1424,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
         <v>58</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1436,7 +1439,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="2" t="s">
         <v>4</v>
       </c>
@@ -1448,7 +1451,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1458,7 +1461,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="2" t="s">
         <v>6</v>
       </c>
@@ -1468,7 +1471,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="2" t="s">
         <v>20</v>
       </c>
@@ -1480,7 +1483,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="2" t="s">
         <v>21</v>
       </c>
@@ -1492,7 +1495,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="2" t="s">
         <v>22</v>
       </c>
@@ -1502,7 +1505,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="10"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
@@ -1512,385 +1515,397 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>0</v>
+      <c r="A19" s="11"/>
+      <c r="B19" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D19" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="10"/>
-      <c r="B20" s="6" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="11"/>
+      <c r="B21" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
-      <c r="B21" s="6" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="11"/>
+      <c r="B22" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="10"/>
-      <c r="B22" s="6" t="s">
-        <v>6</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="11"/>
+      <c r="B23" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="10"/>
-      <c r="B23" s="6" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="11"/>
+      <c r="B24" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="10"/>
-      <c r="B24" s="6" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="11"/>
+      <c r="B25" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="10"/>
-      <c r="B25" s="6" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="11"/>
+      <c r="B26" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="10"/>
-      <c r="B26" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="11"/>
+      <c r="B27" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="10"/>
-      <c r="B27" s="6" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="11"/>
+      <c r="B28" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="9" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B29" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D29" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="9"/>
-      <c r="B29" s="6" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="10"/>
+      <c r="B30" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D30" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="9"/>
-      <c r="B30" s="6" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="10"/>
+      <c r="B31" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="9"/>
-      <c r="B31" s="6" t="s">
-        <v>6</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="10"/>
+      <c r="B32" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="9"/>
-      <c r="B32" s="6" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="10"/>
+      <c r="B33" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D33" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="9"/>
-      <c r="B33" s="6" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="10"/>
+      <c r="B34" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="9"/>
-      <c r="B34" s="6" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="10"/>
+      <c r="B35" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="9"/>
-      <c r="B35" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="10"/>
+      <c r="B36" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="10" t="s">
+    <row r="37" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B37" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D37" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="10"/>
-      <c r="B37" s="6" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="11"/>
+      <c r="B38" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D38" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="10"/>
-      <c r="B38" s="6" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="11"/>
+      <c r="B39" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="10"/>
-      <c r="B39" s="6" t="s">
-        <v>6</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="11"/>
+      <c r="B40" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="10"/>
-      <c r="B40" s="6" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="11"/>
+      <c r="B41" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="10"/>
-      <c r="B41" s="6" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="11"/>
+      <c r="B42" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D42" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="10"/>
-      <c r="B42" s="6" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="11"/>
+      <c r="B43" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="10"/>
-      <c r="B43" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="11"/>
+      <c r="B44" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" s="2"/>
+      <c r="D44" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="10" t="s">
+    <row r="45" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B45" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D45" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="10"/>
-      <c r="B45" s="6" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="11"/>
+      <c r="B46" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D46" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="10"/>
-      <c r="B46" s="6" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="11"/>
+      <c r="B47" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="C46" s="2"/>
-      <c r="D46" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="10"/>
-      <c r="B47" s="6" t="s">
-        <v>6</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="11"/>
+      <c r="B48" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="10"/>
-      <c r="B48" s="6" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="11"/>
+      <c r="B49" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D49" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="10"/>
-      <c r="B49" s="6" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="11"/>
+      <c r="B50" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D50" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="10"/>
-      <c r="B50" s="6" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="11"/>
+      <c r="B51" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="C50" s="2"/>
-      <c r="D50" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="10"/>
-      <c r="B51" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="11"/>
+      <c r="B52" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="3" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A2:A10"/>
-    <mergeCell ref="A19:A27"/>
-    <mergeCell ref="A28:A35"/>
-    <mergeCell ref="A36:A43"/>
-    <mergeCell ref="A44:A51"/>
-    <mergeCell ref="A11:A18"/>
+    <mergeCell ref="A20:A28"/>
+    <mergeCell ref="A29:A36"/>
+    <mergeCell ref="A37:A44"/>
+    <mergeCell ref="A45:A52"/>
+    <mergeCell ref="A11:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1898,10 +1913,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B88B17D0-DD2F-430F-ACAA-DE1EF1BF83C0}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1926,7 +1941,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>57</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1940,19 +1955,17 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="10"/>
+      <c r="A3" s="11"/>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>13</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="10"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="2" t="s">
         <v>20</v>
       </c>
@@ -1964,7 +1977,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
@@ -1976,7 +1989,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="2" t="s">
         <v>24</v>
       </c>
@@ -1987,8 +2000,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
         <v>58</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -2002,7 +2015,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
@@ -2014,7 +2027,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
@@ -2026,7 +2039,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
@@ -2038,225 +2051,237 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>0</v>
+      <c r="A11" s="11"/>
+      <c r="B11" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="B12" s="6" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="11"/>
+      <c r="B13" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="6" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
+      <c r="B14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
-      <c r="B14" s="6" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="11"/>
+      <c r="B15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
-      <c r="B15" s="6" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="11"/>
+      <c r="B16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B17" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
-      <c r="B17" s="6" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
+      <c r="B18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="10"/>
-      <c r="B18" s="6" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="11"/>
+      <c r="B19" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
-      <c r="B19" s="6" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="11"/>
+      <c r="B20" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B21" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
-      <c r="B21" s="6" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="11"/>
+      <c r="B22" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="10"/>
-      <c r="B22" s="6" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="11"/>
+      <c r="B23" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="10"/>
-      <c r="B23" s="6" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="11"/>
+      <c r="B24" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C24" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D24" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B25" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="10"/>
-      <c r="B25" s="6" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="11"/>
+      <c r="B26" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C26" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D26" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="10"/>
-      <c r="B26" s="6" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="11"/>
+      <c r="B27" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="10"/>
-      <c r="B27" s="6" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="11"/>
+      <c r="B28" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>53</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A25:A28"/>
     <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A7:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>